<commit_message>
Nuevas bases de datos
</commit_message>
<xml_diff>
--- a/Bases/GDP_countries_cds.xlsx
+++ b/Bases/GDP_countries_cds.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e8b1635bbae8cdf/Documents/Codigo_compartido_Melo/Climate_Change_and_Financial_Stability/Climate-Change-and-Financial-Stability/Bases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{237C2D4A-E790-481F-B78C-18FA486239C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{237C2D4A-E790-481F-B78C-18FA486239C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7FC81C9-9658-4CB6-BC9F-59862604F3D2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{563A30D3-98F6-44A9-865D-ED7766EF781B}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     <author>OECD.Stat</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{C596534E-CA1A-45FD-9BCA-AD345BF89DED}">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{C596534E-CA1A-45FD-9BCA-AD345BF89DED}">
       <text>
         <r>
           <rPr>
@@ -54,7 +54,176 @@
         </r>
       </text>
     </comment>
-    <comment ref="E63" authorId="0" shapeId="0" xr:uid="{60A9E4A9-DFFA-4ACD-9603-D0F8AB91EE73}">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{184A6071-3F95-4000-B7D5-AB54756B342D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>E: Estimated value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{8D677A61-B1ED-45E6-BC75-B7ABDA27ACC5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>E: Estimated value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{7EA958D2-616B-41B4-AA00-F743ABEE2FD3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>E: Estimated value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{AB123B38-DDB8-4463-8BAE-454615AFF4B2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>E: Estimated value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{4F4277EC-3A04-4C19-B53C-B09239BFA4C2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>E: Estimated value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{FBD3B803-A88C-43F2-8B22-095FD53C08C2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>E: Estimated value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{5F11BF65-1444-49E6-8D38-3027A2C1B6BA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>E: Estimated value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{1132675D-E7DD-45B5-9B92-E57A0B6BCBC6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>E: Estimated value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{7F669BC4-7D32-482A-9031-D8597E6A2F0D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>E: Estimated value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{038524E7-0241-4AA6-A13F-679277A39F24}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>E: Estimated value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{C83391CE-919B-4D8F-83ED-95AD55F667BA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>E: Estimated value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{AA663247-3E8B-4638-B1DC-FE80E42952CD}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>E: Estimated value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{8D66F4E1-0FB9-400B-A3F0-000D3720305B}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>E: Estimated value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I63" authorId="0" shapeId="0" xr:uid="{60A9E4A9-DFFA-4ACD-9603-D0F8AB91EE73}">
       <text>
         <r>
           <rPr>
@@ -67,7 +236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E64" authorId="0" shapeId="0" xr:uid="{F8E92BA1-F1FA-493A-BA38-B866D3B6232B}">
+    <comment ref="I64" authorId="0" shapeId="0" xr:uid="{F8E92BA1-F1FA-493A-BA38-B866D3B6232B}">
       <text>
         <r>
           <rPr>
@@ -80,7 +249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E65" authorId="0" shapeId="0" xr:uid="{B2C8EDE7-5C6B-4969-A0F7-0337B7F23D43}">
+    <comment ref="I65" authorId="0" shapeId="0" xr:uid="{B2C8EDE7-5C6B-4969-A0F7-0337B7F23D43}">
       <text>
         <r>
           <rPr>
@@ -93,7 +262,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E66" authorId="0" shapeId="0" xr:uid="{288ABE44-716D-4B54-B32D-A202E2D7FD74}">
+    <comment ref="I66" authorId="0" shapeId="0" xr:uid="{288ABE44-716D-4B54-B32D-A202E2D7FD74}">
       <text>
         <r>
           <rPr>
@@ -106,7 +275,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E67" authorId="0" shapeId="0" xr:uid="{887C9C6D-26CB-4D50-810C-B2E93BAC168D}">
+    <comment ref="I67" authorId="0" shapeId="0" xr:uid="{887C9C6D-26CB-4D50-810C-B2E93BAC168D}">
       <text>
         <r>
           <rPr>
@@ -119,7 +288,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E68" authorId="0" shapeId="0" xr:uid="{BA9F7FC9-B076-40D6-8E70-3D46E87690AC}">
+    <comment ref="I68" authorId="0" shapeId="0" xr:uid="{BA9F7FC9-B076-40D6-8E70-3D46E87690AC}">
       <text>
         <r>
           <rPr>
@@ -132,7 +301,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E69" authorId="0" shapeId="0" xr:uid="{C0F89811-CE91-41C7-84DE-0A36559442BD}">
+    <comment ref="I69" authorId="0" shapeId="0" xr:uid="{C0F89811-CE91-41C7-84DE-0A36559442BD}">
       <text>
         <r>
           <rPr>
@@ -145,7 +314,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E70" authorId="0" shapeId="0" xr:uid="{E3BE6817-1C62-4A82-960B-6E9B572BC0FB}">
+    <comment ref="I70" authorId="0" shapeId="0" xr:uid="{E3BE6817-1C62-4A82-960B-6E9B572BC0FB}">
       <text>
         <r>
           <rPr>
@@ -158,7 +327,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E71" authorId="0" shapeId="0" xr:uid="{17F3287C-336C-4815-AD00-0022F3809A4E}">
+    <comment ref="G71" authorId="0" shapeId="0" xr:uid="{FA247C5E-C3E5-400C-869F-488CB3EF3323}">
       <text>
         <r>
           <rPr>
@@ -171,7 +340,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E72" authorId="0" shapeId="0" xr:uid="{C764F0ED-DE97-4120-A0FE-35E46074B285}">
+    <comment ref="I71" authorId="0" shapeId="0" xr:uid="{17F3287C-336C-4815-AD00-0022F3809A4E}">
       <text>
         <r>
           <rPr>
@@ -184,7 +353,46 @@
         </r>
       </text>
     </comment>
-    <comment ref="E73" authorId="0" shapeId="0" xr:uid="{4E18CDC4-B456-4354-B93E-385B2C2DF386}">
+    <comment ref="G72" authorId="0" shapeId="0" xr:uid="{F81EE1D8-0436-4C1A-8459-BB4D7D23D0E2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>P: Provisional value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I72" authorId="0" shapeId="0" xr:uid="{C764F0ED-DE97-4120-A0FE-35E46074B285}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>P: Provisional value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G73" authorId="0" shapeId="0" xr:uid="{4CF9ACA7-DBDE-4A1E-BC7F-5FEDAFB8F70E}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>P: Provisional value</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I73" authorId="0" shapeId="0" xr:uid="{4E18CDC4-B456-4354-B93E-385B2C2DF386}">
       <text>
         <r>
           <rPr>
@@ -202,7 +410,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
   <si>
     <t>2004Q4</t>
   </si>
@@ -402,9 +610,6 @@
     <t>Colombia</t>
   </si>
   <si>
-    <t>Perú</t>
-  </si>
-  <si>
     <t>2020Q1</t>
   </si>
   <si>
@@ -436,6 +641,216 @@
   </si>
   <si>
     <t>2022Q3</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Korea</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>53480.3</t>
+  </si>
+  <si>
+    <t>59216.8</t>
+  </si>
+  <si>
+    <t>61099.4</t>
+  </si>
+  <si>
+    <t>67399.2</t>
+  </si>
+  <si>
+    <t>59640.3</t>
+  </si>
+  <si>
+    <t>65699.9</t>
+  </si>
+  <si>
+    <t>66919.4</t>
+  </si>
+  <si>
+    <t>72213.3</t>
+  </si>
+  <si>
+    <t>63431.9</t>
+  </si>
+  <si>
+    <t>71090.4</t>
+  </si>
+  <si>
+    <t>74022.5</t>
+  </si>
+  <si>
+    <t>80785.1</t>
+  </si>
+  <si>
+    <t>71168.0</t>
+  </si>
+  <si>
+    <t>78746.9</t>
+  </si>
+  <si>
+    <t>81366.7</t>
+  </si>
+  <si>
+    <t>88821.1</t>
+  </si>
+  <si>
+    <t>98902.8</t>
+  </si>
+  <si>
+    <t>110314.2</t>
+  </si>
+  <si>
+    <t>115223.5</t>
+  </si>
+  <si>
+    <t>127039.6</t>
+  </si>
+  <si>
+    <t>106938.5</t>
+  </si>
+  <si>
+    <t>118757.4</t>
+  </si>
+  <si>
+    <t>123917.0</t>
+  </si>
+  <si>
+    <t>137370.4</t>
+  </si>
+  <si>
+    <t>115342.5</t>
+  </si>
+  <si>
+    <t>127743.9</t>
+  </si>
+  <si>
+    <t>133751.6</t>
+  </si>
+  <si>
+    <t>147965.2</t>
+  </si>
+  <si>
+    <t>124032.7</t>
+  </si>
+  <si>
+    <t>137477.3</t>
+  </si>
+  <si>
+    <t>143448.1</t>
+  </si>
+  <si>
+    <t>158815.7</t>
+  </si>
+  <si>
+    <t>132883.8</t>
+  </si>
+  <si>
+    <t>147275.4</t>
+  </si>
+  <si>
+    <t>153478.9</t>
+  </si>
+  <si>
+    <t>169832.9</t>
+  </si>
+  <si>
+    <t>161760.5</t>
+  </si>
+  <si>
+    <t>179988.0</t>
+  </si>
+  <si>
+    <t>188607.2</t>
+  </si>
+  <si>
+    <t>205680.8</t>
+  </si>
+  <si>
+    <t>173159.5</t>
+  </si>
+  <si>
+    <t>192594.3</t>
+  </si>
+  <si>
+    <t>201648.3</t>
+  </si>
+  <si>
+    <t>219768.2</t>
+  </si>
+  <si>
+    <t>185190.0</t>
+  </si>
+  <si>
+    <t>205905.5</t>
+  </si>
+  <si>
+    <t>215098.8</t>
+  </si>
+  <si>
+    <t>234108.3</t>
+  </si>
+  <si>
+    <t>196802.8</t>
+  </si>
+  <si>
+    <t>218190.6</t>
+  </si>
+  <si>
+    <t>227683.6</t>
+  </si>
+  <si>
+    <t>247627.8</t>
+  </si>
+  <si>
+    <t>183177.8</t>
+  </si>
+  <si>
+    <t>224846.8</t>
+  </si>
+  <si>
+    <t>238702.1</t>
+  </si>
+  <si>
+    <t>263508.9</t>
+  </si>
+  <si>
+    <t>245513.7</t>
+  </si>
+  <si>
+    <t>268481.9</t>
+  </si>
+  <si>
+    <t>278521.0</t>
+  </si>
+  <si>
+    <t>306681.3</t>
+  </si>
+  <si>
+    <t>257286.1</t>
+  </si>
+  <si>
+    <t>269674.4</t>
+  </si>
+  <si>
+    <t>289504.9</t>
   </si>
 </sst>
 </file>
@@ -471,7 +886,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -481,6 +896,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF0F8FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -512,7 +933,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -521,6 +942,7 @@
     <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -835,21 +1257,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11F4FF4D-4576-438E-84C8-6A1A571DB656}">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:L73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>61</v>
       </c>
@@ -859,17 +1285,35 @@
       <c r="C1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -879,17 +1323,35 @@
       <c r="C2" s="2">
         <v>268149.7</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
+        <v>46796.371918927442</v>
+      </c>
+      <c r="E2" s="3">
         <v>392675.8</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="3">
+        <v>1488501.8</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1303883.8999999999</v>
+      </c>
+      <c r="H2" s="3">
+        <v>178621.5</v>
+      </c>
+      <c r="I2" s="2">
         <v>1769619.4</v>
       </c>
-      <c r="F2">
+      <c r="J2">
         <v>66070.504940596802</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K2" s="2">
+        <v>567180.9</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1153489.1000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -899,17 +1361,35 @@
       <c r="C3" s="2">
         <v>268453.09999999998</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
+        <v>41773.325522358915</v>
+      </c>
+      <c r="E3" s="3">
         <v>392528.6</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="3">
+        <v>1500573.9</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1314978.7</v>
+      </c>
+      <c r="H3" s="3">
+        <v>175385.9</v>
+      </c>
+      <c r="I3" s="2">
         <v>1772543.4</v>
       </c>
-      <c r="F3">
+      <c r="J3">
         <v>64340.889412765799</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K3" s="2">
+        <v>572946.9</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1206664.3999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -919,17 +1399,35 @@
       <c r="C4" s="2">
         <v>272911.40000000002</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
+        <v>45288.36373370044</v>
+      </c>
+      <c r="E4" s="3">
         <v>398923.7</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="3">
+        <v>1517758.6</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1339793.2</v>
+      </c>
+      <c r="H4" s="3">
+        <v>179225.8</v>
+      </c>
+      <c r="I4" s="2">
         <v>1777567.3</v>
       </c>
-      <c r="F4">
+      <c r="J4">
         <v>71310.367619886703</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K4" s="2">
+        <v>583228.69999999995</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1211758.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -939,17 +1437,35 @@
       <c r="C5" s="2">
         <v>279546.8</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
+        <v>47642.863715119398</v>
+      </c>
+      <c r="E5" s="3">
         <v>399123</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="3">
+        <v>1534482.8</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1359961.5</v>
+      </c>
+      <c r="H5" s="3">
+        <v>186594.1</v>
+      </c>
+      <c r="I5" s="2">
         <v>1792530.5</v>
       </c>
-      <c r="F5">
+      <c r="J5">
         <v>67229.826186852093</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K5" s="2">
+        <v>591181.69999999995</v>
+      </c>
+      <c r="L5" s="2">
+        <v>1228868.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -959,17 +1475,35 @@
       <c r="C6" s="2">
         <v>282907.90000000002</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
+        <v>52599.122036874447</v>
+      </c>
+      <c r="E6" s="3">
         <v>406705.5</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="3">
+        <v>1556290.3</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1373730.6</v>
+      </c>
+      <c r="H6" s="3">
+        <v>188610.7</v>
+      </c>
+      <c r="I6" s="2">
         <v>1822506.6</v>
       </c>
-      <c r="F6">
+      <c r="J6">
         <v>71090.070667286403</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K6" s="2">
+        <v>595138.80000000005</v>
+      </c>
+      <c r="L6" s="2">
+        <v>1269504.3999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -979,17 +1513,35 @@
       <c r="C7" s="2">
         <v>285466.40000000002</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
+        <v>46994.991212653782</v>
+      </c>
+      <c r="E7" s="3">
         <v>415873.9</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="3">
+        <v>1576852.3</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1396247.7</v>
+      </c>
+      <c r="H7" s="3">
+        <v>185262.2</v>
+      </c>
+      <c r="I7" s="2">
         <v>1854518.7</v>
       </c>
-      <c r="F7">
+      <c r="J7">
         <v>69670.764068816206</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K7" s="2">
+        <v>605596.4</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1284041.8999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -999,17 +1551,35 @@
       <c r="C8" s="2">
         <v>291392.09999999998</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
+        <v>51492.869565217399</v>
+      </c>
+      <c r="E8" s="3">
         <v>422323.20000000001</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="3">
+        <v>1596985.4</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1406448.7</v>
+      </c>
+      <c r="H8" s="3">
+        <v>189333</v>
+      </c>
+      <c r="I8" s="2">
         <v>1872606.5</v>
       </c>
-      <c r="F8">
+      <c r="J8">
         <v>75823.935493798606</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K8" s="2">
+        <v>614197.4</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1323155.3999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1019,17 +1589,35 @@
       <c r="C9" s="2">
         <v>295359</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
+        <v>53455.293088363956</v>
+      </c>
+      <c r="E9" s="3">
         <v>429723</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="3">
+        <v>1622727.1</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1429148.2</v>
+      </c>
+      <c r="H9" s="3">
+        <v>197257.1</v>
+      </c>
+      <c r="I9" s="2">
         <v>1877757.1</v>
       </c>
-      <c r="F9">
+      <c r="J9">
         <v>72806.269064419306</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K9" s="2">
+        <v>622680.4</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1313185.6000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -1039,17 +1627,35 @@
       <c r="C10" s="2">
         <v>301664.40000000002</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
+        <v>59174.012291483756</v>
+      </c>
+      <c r="E10" s="3">
         <v>436648.1</v>
       </c>
-      <c r="E10" s="2">
+      <c r="F10" s="3">
+        <v>1648599.6</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1440286.3</v>
+      </c>
+      <c r="H10" s="3">
+        <v>198721.9</v>
+      </c>
+      <c r="I10" s="2">
         <v>1882444.2</v>
       </c>
-      <c r="F10">
+      <c r="J10">
         <v>76296.862183394507</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K10" s="2">
+        <v>631290.9</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1342846.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1059,17 +1665,35 @@
       <c r="C11" s="2">
         <v>304759.59999999998</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="3">
         <v>444050.5</v>
       </c>
-      <c r="E11" s="2">
+      <c r="F11" s="3">
+        <v>1675411.8</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1464397.4</v>
+      </c>
+      <c r="H11" s="3">
+        <v>194823</v>
+      </c>
+      <c r="I11" s="2">
         <v>1895730.1</v>
       </c>
-      <c r="F11">
+      <c r="J11">
         <v>73354.118000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K11" s="2">
+        <v>641541</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1367327.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1079,17 +1703,35 @@
       <c r="C12" s="2">
         <v>307858.09999999998</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="3">
         <v>450949.5</v>
       </c>
-      <c r="E12" s="2">
+      <c r="F12" s="3">
+        <v>1703335.9</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1489735.7</v>
+      </c>
+      <c r="H12" s="3">
+        <v>200576.1</v>
+      </c>
+      <c r="I12" s="2">
         <v>1910253</v>
       </c>
-      <c r="F12">
+      <c r="J12">
         <v>80625.952999999994</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K12" s="2">
+        <v>646798.80000000005</v>
+      </c>
+      <c r="L12" s="2">
+        <v>1367745.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -1099,17 +1741,35 @@
       <c r="C13" s="2">
         <v>308704.5</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="3">
         <v>459131.4</v>
       </c>
-      <c r="E13" s="2">
+      <c r="F13" s="3">
+        <v>1730190.1</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1507222.7</v>
+      </c>
+      <c r="H13" s="3">
+        <v>209956.9</v>
+      </c>
+      <c r="I13" s="2">
         <v>1922274.9</v>
       </c>
-      <c r="F13">
+      <c r="J13">
         <v>80699.631999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K13" s="2">
+        <v>654378.9</v>
+      </c>
+      <c r="L13" s="2">
+        <v>1375765.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -1119,17 +1779,35 @@
       <c r="C14" s="2">
         <v>314507.40000000002</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="3">
         <v>465293.8</v>
       </c>
-      <c r="E14" s="2">
+      <c r="F14" s="3">
+        <v>1745173.8</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1539732.7</v>
+      </c>
+      <c r="H14" s="3">
+        <v>213756.5</v>
+      </c>
+      <c r="I14" s="2">
         <v>1929838.6</v>
       </c>
-      <c r="F14">
+      <c r="J14">
         <v>85013.297000000006</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K14" s="2">
+        <v>663651.9</v>
+      </c>
+      <c r="L14" s="2">
+        <v>1422990.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -1139,17 +1817,35 @@
       <c r="C15" s="2">
         <v>321134.90000000002</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="3">
         <v>466579.9</v>
       </c>
-      <c r="E15" s="2">
+      <c r="F15" s="3">
+        <v>1783162.8</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1545928.5</v>
+      </c>
+      <c r="H15" s="3">
+        <v>209638.7</v>
+      </c>
+      <c r="I15" s="2">
         <v>1926338.9</v>
       </c>
-      <c r="F15">
+      <c r="J15">
         <v>80792.367925221595</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K15" s="2">
+        <v>666439.30000000005</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1452965.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -1159,17 +1855,35 @@
       <c r="C16" s="2">
         <v>321451.90000000002</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E16" s="3">
         <v>470282.3</v>
       </c>
-      <c r="E16" s="2">
+      <c r="F16" s="3">
+        <v>1810173.7</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1554021</v>
+      </c>
+      <c r="H16" s="3">
+        <v>213859.9</v>
+      </c>
+      <c r="I16" s="2">
         <v>1940527.4</v>
       </c>
-      <c r="F16">
+      <c r="J16">
         <v>89107.914721936293</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K16" s="2">
+        <v>674575.8</v>
+      </c>
+      <c r="L16" s="2">
+        <v>1401405.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -1179,17 +1893,35 @@
       <c r="C17" s="2">
         <v>318832.5</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="3">
         <v>475266.3</v>
       </c>
-      <c r="E17" s="2">
+      <c r="F17" s="3">
+        <v>1835122.8</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1566700</v>
+      </c>
+      <c r="H17" s="3">
+        <v>220736.8</v>
+      </c>
+      <c r="I17" s="2">
         <v>1946961.3</v>
       </c>
-      <c r="F17">
+      <c r="J17">
         <v>88428.033252541005</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K17" s="2">
+        <v>676187.6</v>
+      </c>
+      <c r="L17" s="2">
+        <v>1375943.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1199,17 +1931,35 @@
       <c r="C18" s="2">
         <v>316272.09999999998</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="3">
         <v>467036.5</v>
       </c>
-      <c r="E18" s="2">
+      <c r="F18" s="3">
+        <v>1837838.1</v>
+      </c>
+      <c r="G18" s="2">
+        <v>1515251.3</v>
+      </c>
+      <c r="H18" s="3">
+        <v>214456</v>
+      </c>
+      <c r="I18" s="2">
         <v>1915172.1</v>
       </c>
-      <c r="F18">
+      <c r="J18">
         <v>90517.748750085695</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K18" s="2">
+        <v>672338.4</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1340994.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -1219,17 +1969,35 @@
       <c r="C19" s="2">
         <v>314733.90000000002</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="3">
         <v>468665.3</v>
       </c>
-      <c r="E19" s="2">
+      <c r="F19" s="3">
+        <v>1862776.4</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1516614.8</v>
+      </c>
+      <c r="H19" s="3">
+        <v>197571.3</v>
+      </c>
+      <c r="I19" s="2">
         <v>1817253.6</v>
       </c>
-      <c r="F19">
+      <c r="J19">
         <v>82889.151996689703</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K19" s="2">
+        <v>661879.9</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1265040.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -1239,17 +2007,35 @@
       <c r="C20" s="2">
         <v>312901</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20" s="3">
         <v>473461.6</v>
       </c>
-      <c r="E20" s="2">
+      <c r="F20" s="3">
+        <v>1886215.7</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1536827.9</v>
+      </c>
+      <c r="H20" s="3">
+        <v>205853.9</v>
+      </c>
+      <c r="I20" s="2">
         <v>1790020.5</v>
       </c>
-      <c r="F20">
+      <c r="J20">
         <v>88453.932566581905</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K20" s="2">
+        <v>659608.19999999995</v>
+      </c>
+      <c r="L20" s="2">
+        <v>1315730.3999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -1259,17 +2045,35 @@
       <c r="C21" s="2">
         <v>316644.5</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="3">
         <v>477274.8</v>
       </c>
-      <c r="E21" s="2">
+      <c r="F21" s="3">
+        <v>1915490.4</v>
+      </c>
+      <c r="G21" s="2">
+        <v>1582820.2</v>
+      </c>
+      <c r="H21" s="3">
+        <v>218250.3</v>
+      </c>
+      <c r="I21" s="2">
         <v>1849276.3</v>
       </c>
-      <c r="F21">
+      <c r="J21">
         <v>88339.057862082904</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K21" s="2">
+        <v>661137.9</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1347252.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1279,17 +2083,35 @@
       <c r="C22" s="2">
         <v>320539.3</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="3">
         <v>481179.3</v>
       </c>
-      <c r="E22" s="2">
+      <c r="F22" s="3">
+        <v>1943459.5</v>
+      </c>
+      <c r="G22" s="2">
+        <v>1594641.7</v>
+      </c>
+      <c r="H22" s="3">
+        <v>224018.1</v>
+      </c>
+      <c r="I22" s="2">
         <v>1879917.8</v>
       </c>
-      <c r="F22">
+      <c r="J22">
         <v>92987.912074786902</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K22" s="2">
+        <v>665547.5</v>
+      </c>
+      <c r="L22" s="2">
+        <v>1373555.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1299,17 +2121,35 @@
       <c r="C23" s="2">
         <v>321576.2</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="3">
         <v>486313</v>
       </c>
-      <c r="E23" s="2">
+      <c r="F23" s="3">
+        <v>1975261.7</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1625882</v>
+      </c>
+      <c r="H23" s="3">
+        <v>217893.1</v>
+      </c>
+      <c r="I23" s="2">
         <v>1899755.3</v>
       </c>
-      <c r="F23">
+      <c r="J23">
         <v>87433.277540164607</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K23" s="2">
+        <v>673312.6</v>
+      </c>
+      <c r="L23" s="2">
+        <v>1369503.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -1319,17 +2159,35 @@
       <c r="C24" s="2">
         <v>332488.7</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" s="3">
         <v>494105</v>
       </c>
-      <c r="E24" s="2">
+      <c r="F24" s="3">
+        <v>2008339.5</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1656770.5</v>
+      </c>
+      <c r="H24" s="3">
+        <v>224551.9</v>
+      </c>
+      <c r="I24" s="2">
         <v>1920427.1</v>
       </c>
-      <c r="F24">
+      <c r="J24">
         <v>96785.709887258403</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K24" s="2">
+        <v>678964.5</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1421554.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1339,17 +2197,35 @@
       <c r="C25" s="2">
         <v>340293.5</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" s="3">
         <v>497390.9</v>
       </c>
-      <c r="E25" s="2">
+      <c r="F25" s="3">
+        <v>2038408.2</v>
+      </c>
+      <c r="G25" s="2">
+        <v>1675909.8</v>
+      </c>
+      <c r="H25" s="3">
+        <v>230851</v>
+      </c>
+      <c r="I25" s="2">
         <v>1938711.7</v>
       </c>
-      <c r="F25">
+      <c r="J25">
         <v>96792.351852670603</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K25" s="2">
+        <v>685008.9</v>
+      </c>
+      <c r="L25" s="2">
+        <v>1460941.3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -1359,17 +2235,35 @@
       <c r="C26" s="2">
         <v>344342.5</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="3">
         <v>508196.8</v>
       </c>
-      <c r="E26" s="2">
+      <c r="F26" s="3">
+        <v>2071138.6</v>
+      </c>
+      <c r="G26" s="2">
+        <v>1696344.5</v>
+      </c>
+      <c r="H26" s="3">
+        <v>236060.7</v>
+      </c>
+      <c r="I26" s="2">
         <v>1953616.2</v>
       </c>
-      <c r="F26">
+      <c r="J26">
         <v>101052.38023296501</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K26" s="2">
+        <v>691384.9</v>
+      </c>
+      <c r="L26" s="2">
+        <v>1505108.3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -1379,17 +2273,35 @@
       <c r="C27" s="2">
         <v>348356.3</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E27" s="3">
         <v>518502</v>
       </c>
-      <c r="E27" s="2">
+      <c r="F27" s="3">
+        <v>2101141.9</v>
+      </c>
+      <c r="G27" s="2">
+        <v>1712173.6</v>
+      </c>
+      <c r="H27" s="3">
+        <v>228798.5</v>
+      </c>
+      <c r="I27" s="2">
         <v>1968588</v>
       </c>
-      <c r="F27">
+      <c r="J27">
         <v>94788.464758230097</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K27" s="2">
+        <v>698193.7</v>
+      </c>
+      <c r="L27" s="2">
+        <v>1539031.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -1399,17 +2311,35 @@
       <c r="C28" s="2">
         <v>353361.5</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" s="3">
         <v>526681.9</v>
       </c>
-      <c r="E28" s="2">
+      <c r="F28" s="3">
+        <v>2131719.2999999998</v>
+      </c>
+      <c r="G28" s="2">
+        <v>1720576.8</v>
+      </c>
+      <c r="H28" s="3">
+        <v>234952.5</v>
+      </c>
+      <c r="I28" s="2">
         <v>1978973.3</v>
       </c>
-      <c r="F28">
+      <c r="J28">
         <v>101898.019726759</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K28" s="2">
+        <v>702101.2</v>
+      </c>
+      <c r="L28" s="2">
+        <v>1581319.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1419,17 +2349,35 @@
       <c r="C29" s="2">
         <v>355628</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E29" s="3">
         <v>537051.1</v>
       </c>
-      <c r="E29" s="2">
+      <c r="F29" s="3">
+        <v>2163952.5</v>
+      </c>
+      <c r="G29" s="2">
+        <v>1729632.6</v>
+      </c>
+      <c r="H29" s="3">
+        <v>244706.6</v>
+      </c>
+      <c r="I29" s="2">
         <v>2017486.8</v>
       </c>
-      <c r="F29">
+      <c r="J29">
         <v>102416.544670588</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K29" s="2">
+        <v>705006.3</v>
+      </c>
+      <c r="L29" s="2">
+        <v>1623364</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1439,17 +2387,35 @@
       <c r="C30" s="2">
         <v>363362.4</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" s="3">
         <v>541756.19999999995</v>
       </c>
-      <c r="E30" s="2">
+      <c r="F30" s="3">
+        <v>2195664</v>
+      </c>
+      <c r="G30" s="2">
+        <v>1737801.6</v>
+      </c>
+      <c r="H30" s="3">
+        <v>249038.4</v>
+      </c>
+      <c r="I30" s="2">
         <v>2030628.8</v>
       </c>
-      <c r="F30">
+      <c r="J30">
         <v>107124.993714011</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K30" s="2">
+        <v>709829.2</v>
+      </c>
+      <c r="L30" s="2">
+        <v>1645398.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -1459,17 +2425,35 @@
       <c r="C31" s="2">
         <v>370830.6</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E31" s="3">
         <v>546224.9</v>
       </c>
-      <c r="E31" s="2">
+      <c r="F31" s="3">
+        <v>2229017.1</v>
+      </c>
+      <c r="G31" s="2">
+        <v>1752845.2</v>
+      </c>
+      <c r="H31" s="3">
+        <v>240422.39999999999</v>
+      </c>
+      <c r="I31" s="2">
         <v>2044026.8</v>
       </c>
-      <c r="F31">
+      <c r="J31">
         <v>100582.471835987</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K31" s="2">
+        <v>713852.8</v>
+      </c>
+      <c r="L31" s="2">
+        <v>1630757.7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -1479,17 +2463,35 @@
       <c r="C32" s="2">
         <v>377704.1</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E32" s="3">
         <v>553205.4</v>
       </c>
-      <c r="E32" s="2">
+      <c r="F32" s="3">
+        <v>2262233.9</v>
+      </c>
+      <c r="G32" s="2">
+        <v>1762765.8</v>
+      </c>
+      <c r="H32" s="3">
+        <v>247282.7</v>
+      </c>
+      <c r="I32" s="2">
         <v>2062055.6</v>
       </c>
-      <c r="F32">
+      <c r="J32">
         <v>107907.29028694201</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K32" s="2">
+        <v>719811.6</v>
+      </c>
+      <c r="L32" s="2">
+        <v>1658929.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -1499,17 +2501,35 @@
       <c r="C33" s="2">
         <v>380639.3</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E33" s="3">
         <v>550345.5</v>
       </c>
-      <c r="E33" s="2">
+      <c r="F33" s="3">
+        <v>2293854.2999999998</v>
+      </c>
+      <c r="G33" s="2">
+        <v>1770729.6</v>
+      </c>
+      <c r="H33" s="3">
+        <v>256963.7</v>
+      </c>
+      <c r="I33" s="2">
         <v>2073106.3</v>
       </c>
-      <c r="F33">
+      <c r="J33">
         <v>109606.954953101</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K33" s="2">
+        <v>722738</v>
+      </c>
+      <c r="L33" s="2">
+        <v>1688206.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -1519,17 +2539,35 @@
       <c r="C34" s="2">
         <v>382898.9</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E34" s="3">
         <v>557319.30000000005</v>
       </c>
-      <c r="E34" s="2">
+      <c r="F34" s="3">
+        <v>2325503.2999999998</v>
+      </c>
+      <c r="G34" s="2">
+        <v>1779623</v>
+      </c>
+      <c r="H34" s="3">
+        <v>265235.5</v>
+      </c>
+      <c r="I34" s="2">
         <v>2090974.5</v>
       </c>
-      <c r="F34">
+      <c r="J34">
         <v>113083.466049882</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K34" s="2">
+        <v>726185.1</v>
+      </c>
+      <c r="L34" s="2">
+        <v>1715266.3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -1539,17 +2577,35 @@
       <c r="C35" s="2">
         <v>386046.6</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E35" s="3">
         <v>565450.6</v>
       </c>
-      <c r="E35" s="2">
+      <c r="F35" s="3">
+        <v>2358077.7999999998</v>
+      </c>
+      <c r="G35" s="2">
+        <v>1794917.6</v>
+      </c>
+      <c r="H35" s="3">
+        <v>250827.4</v>
+      </c>
+      <c r="I35" s="2">
         <v>2096364.3</v>
       </c>
-      <c r="F35">
+      <c r="J35">
         <v>105589.199376783</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K35" s="2">
+        <v>731820.4</v>
+      </c>
+      <c r="L35" s="2">
+        <v>1765521.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -1559,17 +2615,35 @@
       <c r="C36" s="2">
         <v>389457.2</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E36" s="3">
         <v>579731.4</v>
       </c>
-      <c r="E36" s="2">
+      <c r="F36" s="3">
+        <v>2388419.1</v>
+      </c>
+      <c r="G36" s="2">
+        <v>1815849.1</v>
+      </c>
+      <c r="H36" s="3">
+        <v>258549</v>
+      </c>
+      <c r="I36" s="2">
         <v>2085280.7</v>
       </c>
-      <c r="F36">
+      <c r="J36">
         <v>114667.733157401</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K36" s="2">
+        <v>737143.6</v>
+      </c>
+      <c r="L36" s="2">
+        <v>1817353.4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -1579,17 +2653,35 @@
       <c r="C37" s="2">
         <v>391913.5</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E37" s="3">
         <v>583046.5</v>
       </c>
-      <c r="E37" s="2">
+      <c r="F37" s="3">
+        <v>2419837.1</v>
+      </c>
+      <c r="G37" s="2">
+        <v>1831395.5</v>
+      </c>
+      <c r="H37" s="3">
+        <v>269560.59999999998</v>
+      </c>
+      <c r="I37" s="2">
         <v>2103402.1</v>
       </c>
-      <c r="F37">
+      <c r="J37">
         <v>115335.70467237099</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K37" s="2">
+        <v>740641</v>
+      </c>
+      <c r="L37" s="2">
+        <v>1843995.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -1599,17 +2691,35 @@
       <c r="C38" s="2">
         <v>392969.1</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E38" s="3">
         <v>592178.80000000005</v>
       </c>
-      <c r="E38" s="2">
+      <c r="F38" s="3">
+        <v>2450575.2000000002</v>
+      </c>
+      <c r="G38" s="2">
+        <v>1847418.6</v>
+      </c>
+      <c r="H38" s="3">
+        <v>278369.3</v>
+      </c>
+      <c r="I38" s="2">
         <v>2115846.4</v>
       </c>
-      <c r="F38">
+      <c r="J38">
         <v>120819.087282704</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K38" s="2">
+        <v>744628.3</v>
+      </c>
+      <c r="L38" s="2">
+        <v>1847569.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -1619,17 +2729,35 @@
       <c r="C39" s="2">
         <v>394242.3</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E39" s="3">
         <v>599668.19999999995</v>
       </c>
-      <c r="E39" s="2">
+      <c r="F39" s="3">
+        <v>2479504.5</v>
+      </c>
+      <c r="G39" s="2">
+        <v>1863240.8</v>
+      </c>
+      <c r="H39" s="3">
+        <v>266541.8</v>
+      </c>
+      <c r="I39" s="2">
         <v>2130498</v>
       </c>
-      <c r="F39">
+      <c r="J39">
         <v>110822.52456479501</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K39" s="2">
+        <v>743601.2</v>
+      </c>
+      <c r="L39" s="2">
+        <v>1901169</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -1639,17 +2767,35 @@
       <c r="C40" s="2">
         <v>397470.4</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E40" s="3">
         <v>602788.6</v>
       </c>
-      <c r="E40" s="2">
+      <c r="F40" s="3">
+        <v>2510403.7999999998</v>
+      </c>
+      <c r="G40" s="2">
+        <v>1879480.8</v>
+      </c>
+      <c r="H40" s="3">
+        <v>275425.7</v>
+      </c>
+      <c r="I40" s="2">
         <v>2158521.7999999998</v>
       </c>
-      <c r="F40">
+      <c r="J40">
         <v>116915.37710281</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K40" s="2">
+        <v>746535.9</v>
+      </c>
+      <c r="L40" s="2">
+        <v>1870324.3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -1659,17 +2805,35 @@
       <c r="C41" s="2">
         <v>395712.8</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E41" s="3">
         <v>607694.1</v>
       </c>
-      <c r="E41" s="2">
+      <c r="F41" s="3">
+        <v>2539713.2999999998</v>
+      </c>
+      <c r="G41" s="2">
+        <v>1885484.9</v>
+      </c>
+      <c r="H41" s="3">
+        <v>284734.8</v>
+      </c>
+      <c r="I41" s="2">
         <v>2163834.7999999998</v>
       </c>
-      <c r="F41">
+      <c r="J41">
         <v>117439.17286977</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K41" s="2">
+        <v>750123.6</v>
+      </c>
+      <c r="L41" s="2">
+        <v>1916300.3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -1679,17 +2843,35 @@
       <c r="C42" s="2">
         <v>399917</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E42" s="3">
         <v>614652.19999999995</v>
       </c>
-      <c r="E42" s="2">
+      <c r="F42" s="3">
+        <v>2568774.2999999998</v>
+      </c>
+      <c r="G42" s="2">
+        <v>1894819.7</v>
+      </c>
+      <c r="H42" s="3">
+        <v>294112.40000000002</v>
+      </c>
+      <c r="I42" s="2">
         <v>2187953.4</v>
       </c>
-      <c r="F42">
+      <c r="J42">
         <v>122114.101794656</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K42" s="2">
+        <v>755740.3</v>
+      </c>
+      <c r="L42" s="2">
+        <v>1942123.6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -1699,17 +2881,35 @@
       <c r="C43" s="2">
         <v>402627.7</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E43" s="3">
         <v>616985</v>
       </c>
-      <c r="E43" s="2">
+      <c r="F43" s="3">
+        <v>2600237.4</v>
+      </c>
+      <c r="G43" s="2">
+        <v>1909251.2</v>
+      </c>
+      <c r="H43" s="3">
+        <v>282255</v>
+      </c>
+      <c r="I43" s="2">
         <v>2200005.7999999998</v>
       </c>
-      <c r="F43">
+      <c r="J43">
         <v>112960.26194944201</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K43" s="2">
+        <v>761199.5</v>
+      </c>
+      <c r="L43" s="2">
+        <v>1978844.3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -1719,17 +2919,35 @@
       <c r="C44" s="2">
         <v>406357.1</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E44" s="3">
         <v>623475</v>
       </c>
-      <c r="E44" s="2">
+      <c r="F44" s="3">
+        <v>2630243.7999999998</v>
+      </c>
+      <c r="G44" s="2">
+        <v>1918532.8</v>
+      </c>
+      <c r="H44" s="3">
+        <v>288975</v>
+      </c>
+      <c r="I44" s="2">
         <v>2226701.7000000002</v>
       </c>
-      <c r="F44">
+      <c r="J44">
         <v>120623.990275574</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K44" s="2">
+        <v>754772.9</v>
+      </c>
+      <c r="L44" s="2">
+        <v>2008997.3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -1739,17 +2957,35 @@
       <c r="C45" s="2">
         <v>404938.1</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E45" s="3">
         <v>628044</v>
       </c>
-      <c r="E45" s="2">
+      <c r="F45" s="3">
+        <v>2662937.5</v>
+      </c>
+      <c r="G45" s="2">
+        <v>1946568.3</v>
+      </c>
+      <c r="H45" s="3">
+        <v>297965</v>
+      </c>
+      <c r="I45" s="2">
         <v>2252745.4</v>
       </c>
-      <c r="F45">
+      <c r="J45">
         <v>121146.06525828999</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K45" s="2">
+        <v>758172.6</v>
+      </c>
+      <c r="L45" s="2">
+        <v>2037153.7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
@@ -1759,17 +2995,35 @@
       <c r="C46" s="2">
         <v>407505.6</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E46" s="3">
         <v>627973.9</v>
       </c>
-      <c r="E46" s="2">
+      <c r="F46" s="3">
+        <v>2697407.5</v>
+      </c>
+      <c r="G46" s="2">
+        <v>1960003.5</v>
+      </c>
+      <c r="H46" s="3">
+        <v>307745</v>
+      </c>
+      <c r="I46" s="2">
         <v>2247699.4</v>
       </c>
-      <c r="F46">
+      <c r="J46">
         <v>127756.199459904</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K46" s="2">
+        <v>761459</v>
+      </c>
+      <c r="L46" s="2">
+        <v>2060924.6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
@@ -1779,17 +3033,35 @@
       <c r="C47" s="2">
         <v>412359.8</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E47" s="3">
         <v>631727.1</v>
       </c>
-      <c r="E47" s="2">
+      <c r="F47" s="3">
+        <v>2729813.2</v>
+      </c>
+      <c r="G47" s="2">
+        <v>1965347</v>
+      </c>
+      <c r="H47" s="3">
+        <v>294329</v>
+      </c>
+      <c r="I47" s="2">
         <v>2260804</v>
       </c>
-      <c r="F47">
+      <c r="J47">
         <v>118029.990107255</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K47" s="2">
+        <v>763277.9</v>
+      </c>
+      <c r="L47" s="2">
+        <v>2068375.6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
@@ -1799,17 +3071,35 @@
       <c r="C48" s="2">
         <v>410377.2</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E48" s="3">
         <v>635597.5</v>
       </c>
-      <c r="E48" s="2">
+      <c r="F48" s="3">
+        <v>2764246.1</v>
+      </c>
+      <c r="G48" s="2">
+        <v>1989570</v>
+      </c>
+      <c r="H48" s="3">
+        <v>301015</v>
+      </c>
+      <c r="I48" s="2">
         <v>2270615.1</v>
       </c>
-      <c r="F48">
+      <c r="J48">
         <v>125145.55270395899</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K48" s="2">
+        <v>764012.3</v>
+      </c>
+      <c r="L48" s="2">
+        <v>2097971.7000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
@@ -1819,17 +3109,35 @@
       <c r="C49" s="2">
         <v>413060.7</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E49" s="3">
         <v>638139.30000000005</v>
       </c>
-      <c r="E49" s="2">
+      <c r="F49" s="3">
+        <v>2798091.1</v>
+      </c>
+      <c r="G49" s="2">
+        <v>1997690.5</v>
+      </c>
+      <c r="H49" s="3">
+        <v>311510</v>
+      </c>
+      <c r="I49" s="2">
         <v>2291272.2999999998</v>
       </c>
-      <c r="F49">
+      <c r="J49">
         <v>126731.476345559</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K49" s="2">
+        <v>763919.2</v>
+      </c>
+      <c r="L49" s="2">
+        <v>2037808.7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
@@ -1839,17 +3147,35 @@
       <c r="C50" s="2">
         <v>412347.7</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E50" s="3">
         <v>643125</v>
       </c>
-      <c r="E50" s="2">
+      <c r="F50" s="3">
+        <v>2831719.4</v>
+      </c>
+      <c r="G50" s="2">
+        <v>2009670.7</v>
+      </c>
+      <c r="H50" s="3">
+        <v>322458</v>
+      </c>
+      <c r="I50" s="2">
         <v>2318317.7000000002</v>
       </c>
-      <c r="F50">
+      <c r="J50">
         <v>131656.50692488899</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K50" s="2">
+        <v>764567.9</v>
+      </c>
+      <c r="L50" s="2">
+        <v>2150084.1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
@@ -1859,17 +3185,35 @@
       <c r="C51" s="2">
         <v>409994.9</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E51" s="3">
         <v>641172.6</v>
       </c>
-      <c r="E51" s="2">
+      <c r="F51" s="3">
+        <v>2867301.1</v>
+      </c>
+      <c r="G51" s="2">
+        <v>2029320.2</v>
+      </c>
+      <c r="H51" s="3">
+        <v>310744</v>
+      </c>
+      <c r="I51" s="2">
         <v>2329353.4</v>
       </c>
-      <c r="F51">
+      <c r="J51">
         <v>120740.65399999999</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K51" s="2">
+        <v>768177.6</v>
+      </c>
+      <c r="L51" s="2">
+        <v>2179515.9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
@@ -1879,17 +3223,35 @@
       <c r="C52" s="2">
         <v>415155.3</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E52" s="3">
         <v>644630.4</v>
       </c>
-      <c r="E52" s="2">
+      <c r="F52" s="3">
+        <v>2903186.2</v>
+      </c>
+      <c r="G52" s="2">
+        <v>2044733.3</v>
+      </c>
+      <c r="H52" s="3">
+        <v>318231</v>
+      </c>
+      <c r="I52" s="2">
         <v>2336824.9</v>
       </c>
-      <c r="F52">
+      <c r="J52">
         <v>128455.253</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K52" s="2">
+        <v>772366.5</v>
+      </c>
+      <c r="L52" s="2">
+        <v>2229215.7999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
@@ -1899,17 +3261,35 @@
       <c r="C53" s="2">
         <v>423151.1</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E53" s="3">
         <v>646418.80000000005</v>
       </c>
-      <c r="E53" s="2">
+      <c r="F53" s="3">
+        <v>2939822.8</v>
+      </c>
+      <c r="G53" s="2">
+        <v>2073255.8</v>
+      </c>
+      <c r="H53" s="3">
+        <v>330664</v>
+      </c>
+      <c r="I53" s="2">
         <v>2327213.4</v>
       </c>
-      <c r="F53">
+      <c r="J53">
         <v>130293.94</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K53" s="2">
+        <v>773786.8</v>
+      </c>
+      <c r="L53" s="2">
+        <v>2263008.9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
@@ -1919,17 +3299,35 @@
       <c r="C54" s="2">
         <v>426046</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E54" s="3">
         <v>651011.6</v>
       </c>
-      <c r="E54" s="2">
+      <c r="F54" s="3">
+        <v>2977516.2</v>
+      </c>
+      <c r="G54" s="2">
+        <v>2066547.8</v>
+      </c>
+      <c r="H54" s="3">
+        <v>341129</v>
+      </c>
+      <c r="I54" s="2">
         <v>2361069.2000000002</v>
       </c>
-      <c r="F54">
+      <c r="J54">
         <v>134725.15299999999</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K54" s="2">
+        <v>776830.6</v>
+      </c>
+      <c r="L54" s="2">
+        <v>2305615.9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
@@ -1939,17 +3337,35 @@
       <c r="C55" s="2">
         <v>430504</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D55" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E55" s="3">
         <v>655067.9</v>
       </c>
-      <c r="E55" s="2">
+      <c r="F55" s="3">
+        <v>3015738.2</v>
+      </c>
+      <c r="G55" s="2">
+        <v>2092455.7</v>
+      </c>
+      <c r="H55" s="3">
+        <v>327096</v>
+      </c>
+      <c r="I55" s="2">
         <v>2387925.6</v>
       </c>
-      <c r="F55">
+      <c r="J55">
         <v>124547.622</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K55" s="2">
+        <v>780940.2</v>
+      </c>
+      <c r="L55" s="2">
+        <v>2339479.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
@@ -1959,17 +3375,35 @@
       <c r="C56" s="2">
         <v>436343</v>
       </c>
-      <c r="D56" s="3">
+      <c r="D56" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E56" s="3">
         <v>658897.30000000005</v>
       </c>
-      <c r="E56" s="2">
+      <c r="F56" s="3">
+        <v>3053489</v>
+      </c>
+      <c r="G56" s="2">
+        <v>2106856.9</v>
+      </c>
+      <c r="H56" s="3">
+        <v>333438</v>
+      </c>
+      <c r="I56" s="2">
         <v>2386244</v>
       </c>
-      <c r="F56">
+      <c r="J56">
         <v>135645.614</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K56" s="2">
+        <v>778998.4</v>
+      </c>
+      <c r="L56" s="2">
+        <v>2354862.1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
@@ -1979,17 +3413,35 @@
       <c r="C57" s="2">
         <v>434761.2</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D57" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E57" s="3">
         <v>664761.30000000005</v>
       </c>
-      <c r="E57" s="2">
+      <c r="F57" s="3">
+        <v>3092169.4</v>
+      </c>
+      <c r="G57" s="2">
+        <v>2119849.2999999998</v>
+      </c>
+      <c r="H57" s="3">
+        <v>345685</v>
+      </c>
+      <c r="I57" s="2">
         <v>2392817.1</v>
       </c>
-      <c r="F57">
+      <c r="J57">
         <v>133481.75599999999</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K57" s="2">
+        <v>788578.7</v>
+      </c>
+      <c r="L57" s="2">
+        <v>2316526.4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>56</v>
       </c>
@@ -1999,17 +3451,35 @@
       <c r="C58" s="2">
         <v>440066.5</v>
       </c>
-      <c r="D58" s="3">
+      <c r="D58" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E58" s="3">
         <v>670749.4</v>
       </c>
-      <c r="E58" s="2">
+      <c r="F58" s="3">
+        <v>3131191.8</v>
+      </c>
+      <c r="G58" s="2">
+        <v>2133504.7000000002</v>
+      </c>
+      <c r="H58" s="3">
+        <v>357547</v>
+      </c>
+      <c r="I58" s="2">
         <v>2391669.9</v>
       </c>
-      <c r="F58">
+      <c r="J58">
         <v>140951.008</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K58" s="2">
+        <v>790766.9</v>
+      </c>
+      <c r="L58" s="2">
+        <v>2242765.6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
@@ -2019,17 +3489,35 @@
       <c r="C59" s="2">
         <v>438589.9</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D59" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E59" s="3">
         <v>675819.4</v>
       </c>
-      <c r="E59" s="2">
+      <c r="F59" s="3">
+        <v>3169931.3</v>
+      </c>
+      <c r="G59" s="2">
+        <v>2132059.5</v>
+      </c>
+      <c r="H59" s="3">
+        <v>342373</v>
+      </c>
+      <c r="I59" s="2">
         <v>2392802.2999999998</v>
       </c>
-      <c r="F59">
+      <c r="J59">
         <v>127523.85</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K59" s="2">
+        <v>783860.1</v>
+      </c>
+      <c r="L59" s="2">
+        <v>2284880</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
@@ -2039,17 +3527,35 @@
       <c r="C60" s="2">
         <v>443747.3</v>
       </c>
-      <c r="D60" s="3">
+      <c r="D60" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E60" s="3">
         <v>681363.4</v>
       </c>
-      <c r="E60" s="2">
+      <c r="F60" s="3">
+        <v>3209540.3</v>
+      </c>
+      <c r="G60" s="2">
+        <v>2155351.7999999998</v>
+      </c>
+      <c r="H60" s="3">
+        <v>349910</v>
+      </c>
+      <c r="I60" s="2">
         <v>2382639.4</v>
       </c>
-      <c r="F60">
+      <c r="J60">
         <v>137191.76300000001</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K60" s="2">
+        <v>787404.80000000005</v>
+      </c>
+      <c r="L60" s="2">
+        <v>2343551.1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
@@ -2059,17 +3565,35 @@
       <c r="C61" s="2">
         <v>444486.8</v>
       </c>
-      <c r="D61" s="3">
+      <c r="D61" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E61" s="3">
         <v>684870.9</v>
       </c>
-      <c r="E61" s="2">
+      <c r="F61" s="3">
+        <v>3247929.7</v>
+      </c>
+      <c r="G61" s="2">
+        <v>2164303.6</v>
+      </c>
+      <c r="H61" s="3">
+        <v>361117</v>
+      </c>
+      <c r="I61" s="2">
         <v>2388183.2999999998</v>
       </c>
-      <c r="F61">
+      <c r="J61">
         <v>138009.198</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K61" s="2">
+        <v>788232.4</v>
+      </c>
+      <c r="L61" s="2">
+        <v>2335280.6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
@@ -2079,19 +3603,37 @@
       <c r="C62" s="2">
         <v>427105</v>
       </c>
-      <c r="D62" s="3">
+      <c r="D62" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E62" s="3">
         <v>691857.1</v>
       </c>
-      <c r="E62" s="2">
+      <c r="F62" s="3">
+        <v>3282187.4</v>
+      </c>
+      <c r="G62" s="2">
+        <v>2190628.1</v>
+      </c>
+      <c r="H62" s="3">
+        <v>370552</v>
+      </c>
+      <c r="I62" s="2">
         <v>2377223.7999999998</v>
       </c>
-      <c r="F62">
+      <c r="J62">
         <v>143880.18900000001</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K62" s="2">
+        <v>787947</v>
+      </c>
+      <c r="L62" s="2">
+        <v>2365170</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B63" s="3">
         <v>2998457.4</v>
@@ -2099,19 +3641,37 @@
       <c r="C63" s="2">
         <v>438636.2</v>
       </c>
-      <c r="D63" s="3">
+      <c r="D63" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E63" s="3">
         <v>675802.3</v>
       </c>
-      <c r="E63" s="2">
+      <c r="F63" s="3">
+        <v>3261606</v>
+      </c>
+      <c r="G63" s="2">
+        <v>2162670</v>
+      </c>
+      <c r="H63" s="3">
+        <v>344690</v>
+      </c>
+      <c r="I63" s="2">
         <v>2353738.7000000002</v>
       </c>
-      <c r="F63">
+      <c r="J63">
         <v>123063.595</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K63" s="2">
+        <v>789806</v>
+      </c>
+      <c r="L63" s="2">
+        <v>2385258</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B64" s="3">
         <v>2737221.7</v>
@@ -2119,19 +3679,37 @@
       <c r="C64" s="2">
         <v>380602.4</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D64" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E64" s="3">
         <v>567416.1</v>
       </c>
-      <c r="E64" s="2">
+      <c r="F64" s="3">
+        <v>3035423.3</v>
+      </c>
+      <c r="G64" s="2">
+        <v>2097455.4</v>
+      </c>
+      <c r="H64" s="3">
+        <v>290686</v>
+      </c>
+      <c r="I64" s="2">
         <v>1934653.1</v>
       </c>
-      <c r="F64">
+      <c r="J64">
         <v>95967.483999999997</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K64" s="2">
+        <v>656408.30000000005</v>
+      </c>
+      <c r="L64" s="2">
+        <v>2137864.9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B65" s="3">
         <v>2954858.7</v>
@@ -2139,19 +3717,37 @@
       <c r="C65" s="2">
         <v>398596.7</v>
       </c>
-      <c r="D65" s="3">
+      <c r="D65" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E65" s="3">
         <v>622806</v>
       </c>
-      <c r="E65" s="2">
+      <c r="F65" s="3">
+        <v>3135861.8</v>
+      </c>
+      <c r="G65" s="2">
+        <v>2146010.6</v>
+      </c>
+      <c r="H65" s="3">
+        <v>352137</v>
+      </c>
+      <c r="I65" s="2">
         <v>2189355.2999999998</v>
       </c>
-      <c r="F65">
+      <c r="J65">
         <v>125941.44</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K65" s="2">
+        <v>746533.4</v>
+      </c>
+      <c r="L65" s="2">
+        <v>2472426.2000000002</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B66" s="3">
         <v>3054447.9</v>
@@ -2159,19 +3755,37 @@
       <c r="C66" s="2">
         <v>425361.5</v>
       </c>
-      <c r="D66" s="3">
+      <c r="D66" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E66" s="3">
         <v>669615.1</v>
       </c>
-      <c r="E66" s="2">
+      <c r="F66" s="3">
+        <v>3210048.5</v>
+      </c>
+      <c r="G66" s="2">
+        <v>2174896.9</v>
+      </c>
+      <c r="H66" s="3">
+        <v>358736</v>
+      </c>
+      <c r="I66" s="2">
         <v>2284198.2999999998</v>
       </c>
-      <c r="F66">
+      <c r="J66">
         <v>141764.481</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K66" s="2">
+        <v>767003.3</v>
+      </c>
+      <c r="L66" s="2">
+        <v>2499243.2999999998</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B67" s="3">
         <v>3086491.3</v>
@@ -2179,19 +3793,37 @@
       <c r="C67" s="2">
         <v>444237.2</v>
       </c>
-      <c r="D67" s="3">
+      <c r="D67" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E67" s="3">
         <v>692575.2</v>
       </c>
-      <c r="E67" s="2">
+      <c r="F67" s="3">
+        <v>3244013.6</v>
+      </c>
+      <c r="G67" s="2">
+        <v>2213762.2999999998</v>
+      </c>
+      <c r="H67" s="3">
+        <v>344005</v>
+      </c>
+      <c r="I67" s="2">
         <v>2291757.2999999998</v>
       </c>
-      <c r="F67">
+      <c r="J67">
         <v>128265.17</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K67" s="2">
+        <v>771921.6</v>
+      </c>
+      <c r="L67" s="2">
+        <v>2564640</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B68" s="3">
         <v>3077131</v>
@@ -2199,19 +3831,37 @@
       <c r="C68" s="2">
         <v>448501.1</v>
       </c>
-      <c r="D68" s="3">
+      <c r="D68" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E68" s="3">
         <v>673516.5</v>
       </c>
-      <c r="E68" s="2">
+      <c r="F68" s="3">
+        <v>3251943.9</v>
+      </c>
+      <c r="G68" s="2">
+        <v>2233258.4</v>
+      </c>
+      <c r="H68" s="3">
+        <v>337770</v>
+      </c>
+      <c r="I68" s="2">
         <v>2309047.7999999998</v>
       </c>
-      <c r="F68">
+      <c r="J68">
         <v>136398.125</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K68" s="2">
+        <v>781940.1</v>
+      </c>
+      <c r="L68" s="2">
+        <v>2615803.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B69" s="3">
         <v>3086694.8</v>
@@ -2219,19 +3869,37 @@
       <c r="C69" s="2">
         <v>467708.9</v>
       </c>
-      <c r="D69" s="3">
+      <c r="D69" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E69" s="3">
         <v>705589.1</v>
       </c>
-      <c r="E69" s="2">
+      <c r="F69" s="3">
+        <v>3254262.7</v>
+      </c>
+      <c r="G69" s="2">
+        <v>2236099.7999999998</v>
+      </c>
+      <c r="H69" s="3">
+        <v>337286</v>
+      </c>
+      <c r="I69" s="2">
         <v>2283612.2000000002</v>
       </c>
-      <c r="F69">
+      <c r="J69">
         <v>140624.82399999999</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K69" s="2">
+        <v>767276.7</v>
+      </c>
+      <c r="L69" s="2">
+        <v>2686809</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B70" s="3">
         <v>3119445.5</v>
@@ -2239,19 +3907,37 @@
       <c r="C70" s="2">
         <v>478807.5</v>
       </c>
-      <c r="D70" s="3">
+      <c r="D70" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E70" s="3">
         <v>743289.6</v>
       </c>
-      <c r="E70" s="2">
+      <c r="F70" s="3">
+        <v>3360894.5</v>
+      </c>
+      <c r="G70" s="2">
+        <v>2267303.2000000002</v>
+      </c>
+      <c r="H70" s="3">
+        <v>371583</v>
+      </c>
+      <c r="I70" s="2">
         <v>2310597.2999999998</v>
       </c>
-      <c r="F70">
+      <c r="J70">
         <v>146425.88099999999</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K70" s="2">
+        <v>777811.4</v>
+      </c>
+      <c r="L70" s="2">
+        <v>2729143.4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B71" s="3">
         <v>3161033.3</v>
@@ -2259,19 +3945,37 @@
       <c r="C71" s="2">
         <v>475960.6</v>
       </c>
-      <c r="D71" s="3">
+      <c r="D71" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E71" s="3">
         <v>748336.3</v>
       </c>
-      <c r="E71" s="2">
+      <c r="F71" s="3">
+        <v>3394994.4</v>
+      </c>
+      <c r="G71" s="2">
+        <v>2282280</v>
+      </c>
+      <c r="H71" s="3">
+        <v>360603</v>
+      </c>
+      <c r="I71" s="2">
         <v>2334107.2999999998</v>
       </c>
-      <c r="F71">
+      <c r="J71">
         <v>133284.72700000001</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K71" s="2">
+        <v>789728</v>
+      </c>
+      <c r="L71" s="2">
+        <v>2749146</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B72" s="3">
         <v>3189547.7</v>
@@ -2279,19 +3983,37 @@
       <c r="C72" s="2">
         <v>472937.5</v>
       </c>
-      <c r="D72" s="3">
+      <c r="D72" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E72" s="3">
         <v>754706.1</v>
       </c>
-      <c r="E72" s="2">
+      <c r="F72" s="3">
+        <v>3427740.6</v>
+      </c>
+      <c r="G72" s="2">
+        <v>2299407.7999999998</v>
+      </c>
+      <c r="H72" s="3">
+        <v>367444</v>
+      </c>
+      <c r="I72" s="2">
         <v>2359881.2000000002</v>
       </c>
-      <c r="F72">
+      <c r="J72">
         <v>140994.75200000001</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K72" s="2">
+        <v>783119.9</v>
+      </c>
+      <c r="L72" s="2">
+        <v>2799881.8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B73" s="3">
         <v>3198419.3</v>
@@ -2299,14 +4021,32 @@
       <c r="C73" s="2">
         <v>467726.9</v>
       </c>
-      <c r="D73" s="3">
+      <c r="D73" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E73" s="3">
         <v>756635.7</v>
       </c>
-      <c r="E73" s="2">
+      <c r="F73" s="3">
+        <v>3453437.5</v>
+      </c>
+      <c r="G73" s="2">
+        <v>2304782.1</v>
+      </c>
+      <c r="H73" s="3">
+        <v>384884</v>
+      </c>
+      <c r="I73" s="2">
         <v>2381473.5</v>
       </c>
-      <c r="F73">
+      <c r="J73">
         <v>143375.54199999999</v>
+      </c>
+      <c r="K73" s="2">
+        <v>797012.1</v>
+      </c>
+      <c r="L73" s="2">
+        <v>2797627</v>
       </c>
     </row>
   </sheetData>

</xml_diff>